<commit_message>
Support SHA256 digest TemplateVariable transformations.
</commit_message>
<xml_diff>
--- a/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
+++ b/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">pulldata('pets_APP_USER', 'name', 'name', 'carrot')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -266,7 +269,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,136 +562,136 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -730,7 +733,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1743,18 +1753,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2786,37 +2796,37 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="str">
+      <c r="C2" s="1" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250221191511</v>
+        <v>20250228205739</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3843,47 +3853,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Support SHA256 digest TemplateVariable transformations. (#15)
</commit_message>
<xml_diff>
--- a/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
+++ b/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">pulldata('pets_APP_USER', 'name', 'name', 'carrot')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -266,7 +269,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,136 +562,136 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -730,7 +733,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1743,18 +1753,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2786,37 +2796,37 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="str">
+      <c r="C2" s="1" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250221191511</v>
+        <v>20250228205739</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3843,47 +3853,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Change how static attachments are detected in forms.
</commit_message>
<xml_diff>
--- a/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
+++ b/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logo.png</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -270,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,6 +287,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,11 +571,11 @@
   <dimension ref="A1:T987"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T6" activeCellId="0" sqref="T6"/>
+      <selection pane="bottomRight" activeCell="T13" activeCellId="0" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -756,6 +763,9 @@
       </c>
       <c r="B13" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1775,7 +1785,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2821,28 +2831,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250305175701</v>
+        <v>20250305183239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3874,7 +3884,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3882,34 +3892,34 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Support publishing forms with static attachments. (#13)
* Support publishing forms with static attachments.

* Change how static attachments are detected in forms.

* Use a context manager to clean up temp files created for attachments.

* Update set_survey_attachments docstring.
</commit_message>
<xml_diff>
--- a/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
+++ b/tests/odk_publish/etl/transform/ODK XLSForm Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">video</t>
   </si>
   <si>
+    <t xml:space="preserve">media::image</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculate</t>
   </si>
   <si>
@@ -143,6 +146,12 @@
   </si>
   <si>
     <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logo.png</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -264,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,6 +287,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -555,14 +568,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S987"/>
+  <dimension ref="A1:T987"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="T13" activeCellId="0" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -637,111 +650,124 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1759,7 +1785,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2805,28 +2831,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250228205739</v>
+        <v>20250305183239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3858,7 +3884,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3866,34 +3892,34 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>